<commit_message>
add a case-sensitive data in filter.xlsx
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/filter.xlsx
+++ b/src/main/webapp/WEB-INF/books/filter.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CB1099-F96B-0A48-8C54-1F53A5B1B5EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C99B31-80BB-9940-95D9-61DBFE467816}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simple" sheetId="1" r:id="rId1"/>
     <sheet name="monthly report" sheetId="2" r:id="rId2"/>
+    <sheet name="case-sensitive" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'case-sensitive'!$A$1:$A$17</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'monthly report'!$A$3:$F$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">simple!$A$1:$C$11</definedName>
   </definedNames>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Type</t>
   </si>
@@ -87,6 +89,57 @@
   </si>
   <si>
     <t>Quarterly Profit</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>a-1</t>
+  </si>
+  <si>
+    <t>c-3</t>
+  </si>
+  <si>
+    <t>A-1</t>
+  </si>
+  <si>
+    <t>B-2</t>
+  </si>
+  <si>
+    <t>b-2</t>
+  </si>
+  <si>
+    <t>d-4</t>
+  </si>
+  <si>
+    <t>C-3</t>
+  </si>
+  <si>
+    <t>D-4</t>
+  </si>
+  <si>
+    <t>1-a</t>
+  </si>
+  <si>
+    <t>2-b</t>
+  </si>
+  <si>
+    <t>3-c</t>
+  </si>
+  <si>
+    <t>4-d</t>
+  </si>
+  <si>
+    <t>1-A</t>
+  </si>
+  <si>
+    <t>2-B</t>
+  </si>
+  <si>
+    <t>3-C</t>
+  </si>
+  <si>
+    <t>4-D</t>
   </si>
 </sst>
 </file>
@@ -97,7 +150,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +218,14 @@
       <color theme="2" tint="-0.89999084444715716"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -262,7 +323,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -274,9 +335,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -298,6 +356,15 @@
     <xf numFmtId="165" fontId="9" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="9" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 4" xfId="1" builtinId="19"/>
@@ -640,7 +707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -790,313 +857,313 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="15" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="11.1640625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="15" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" ht="21" customHeight="1">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1">
-      <c r="A4" s="12">
+      <c r="A4" s="11">
         <v>42384</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>13</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="13">
         <v>89500</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="13">
         <v>62600</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <f>C4-D4</f>
         <v>26900</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="15">
         <f>E4</f>
         <v>26900</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1">
-      <c r="A5" s="12">
+      <c r="A5" s="11">
         <v>42415</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="12">
         <v>19</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="13">
         <v>100500</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <v>60300</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <f t="shared" ref="E5:E15" si="0">C5-D5</f>
         <v>40200</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="15">
         <f>E4+E5</f>
         <v>67100</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1">
-      <c r="A6" s="12">
+      <c r="A6" s="11">
         <v>42444</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <v>25</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <v>119200</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>27800</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <f t="shared" si="0"/>
         <v>91400</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="15">
         <f>E4+E5+E6</f>
         <v>158500</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1">
-      <c r="A7" s="12">
+      <c r="A7" s="11">
         <v>42475</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <v>22</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>115900</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <v>79600</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <f>C7-D7</f>
         <v>36300</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="16">
         <f>E7</f>
         <v>36300</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" customHeight="1">
-      <c r="A8" s="12">
+      <c r="A8" s="11">
         <v>42505</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <v>28</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <v>123700</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <v>84000</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <f t="shared" si="0"/>
         <v>39700</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="16">
         <f>E7+E8</f>
         <v>76000</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1">
-      <c r="A9" s="12">
+      <c r="A9" s="11">
         <v>42536</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <v>35</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="13">
         <v>129300</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <v>83100</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <f t="shared" si="0"/>
         <v>46200</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="16">
         <f>E7+E8+E9</f>
         <v>122200</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1">
-      <c r="A10" s="12">
+      <c r="A10" s="11">
         <v>42566</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <v>20</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="13">
         <v>110700</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <v>77300</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="14">
         <f t="shared" si="0"/>
         <v>33400</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="17">
         <f>E10</f>
         <v>33400</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" customHeight="1">
-      <c r="A11" s="12">
+      <c r="A11" s="11">
         <v>42597</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <v>31</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="13">
         <v>125100</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="13">
         <v>85500</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="14">
         <f t="shared" si="0"/>
         <v>39600</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="17">
         <f>E10+E11</f>
         <v>73000</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1">
-      <c r="A12" s="12">
+      <c r="A12" s="11">
         <v>42628</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="12">
         <v>27</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="13">
         <v>120100</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="13">
         <v>78900</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="14">
         <f t="shared" si="0"/>
         <v>41200</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="17">
         <f>E10+E11+E12</f>
         <v>114200</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18" customHeight="1">
-      <c r="A13" s="12">
+      <c r="A13" s="11">
         <v>42658</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="12">
         <v>24</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="13">
         <v>118400</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="13">
         <v>91000</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="14">
         <f t="shared" si="0"/>
         <v>27400</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="18">
         <f>E13</f>
         <v>27400</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="18" customHeight="1">
-      <c r="A14" s="12">
+      <c r="A14" s="11">
         <v>42689</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="12">
         <v>19</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="13">
         <v>100300</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="13">
         <v>65100</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="14">
         <f t="shared" si="0"/>
         <v>35200</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="18">
         <f>E13+E14</f>
         <v>62600</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="18" customHeight="1">
-      <c r="A15" s="12">
+      <c r="A15" s="11">
         <v>42719</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="12">
         <v>17</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="13">
         <v>94200</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="13">
         <v>65800</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <f t="shared" si="0"/>
         <v>28400</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="18">
         <f>E13+E14+E15</f>
         <v>91000</v>
       </c>
@@ -1124,4 +1191,103 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2D71B0-48C9-824A-8CB7-87FA03CBD3E8}">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A17" xr:uid="{A003D063-7211-634F-B674-83D51EDB4529}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>